<commit_message>
Added Chamber and Humidity Values
Chamber and Humidity Values for Dog Bone printing
</commit_message>
<xml_diff>
--- a/Randomize-Prints/Tensile-Specimen/Established_Printing_Order.xlsx
+++ b/Randomize-Prints/Tensile-Specimen/Established_Printing_Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berkeley\Documents\GitHub\3D-Filament-Dyes\Randomize-Prints\Tensile-Specimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87AFF9D3-5F0A-4E85-92B6-8DB056C24D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C04707-B57A-4174-BD57-AF10E64D251A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{26A5D843-55D7-43C2-8BE2-8D2709DF1008}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>green_230</t>
   </si>
@@ -61,42 +61,18 @@
     <t>Object 2</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Print Date</t>
   </si>
   <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Chamber Temp</t>
-  </si>
-  <si>
-    <t>Humidity</t>
-  </si>
-  <si>
-    <t>Indoor Humidity</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Mid Print Chamber Temp</t>
-  </si>
-  <si>
     <t>Humidity Mid Print</t>
   </si>
   <si>
     <t>Indoor Humidity Mid Print</t>
   </si>
   <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Finished Chamber Temp</t>
-  </si>
-  <si>
     <t>Finished Humidity</t>
   </si>
   <si>
@@ -106,9 +82,6 @@
     <t>Finish Time</t>
   </si>
   <si>
-    <t>39C</t>
-  </si>
-  <si>
     <t>red_200</t>
   </si>
   <si>
@@ -122,12 +95,30 @@
   </si>
   <si>
     <t>purple_200</t>
+  </si>
+  <si>
+    <t>Initial Humidity [%]</t>
+  </si>
+  <si>
+    <t>Initial Indoor Humidity [%]</t>
+  </si>
+  <si>
+    <t>Initial Chamber Temp [°C]</t>
+  </si>
+  <si>
+    <t>Mid Print Chamber Temp [°C]</t>
+  </si>
+  <si>
+    <t>Finished Chamber Temp [°C]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="[$-409]h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +433,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -561,7 +564,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -604,15 +607,37 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -652,6 +677,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -986,246 +1012,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A11E65-A701-4B10-AC3C-D4F7CE4948E4}">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="6" max="6" width="12.69140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="12.69140625" customWidth="1"/>
+    <col min="8" max="9" width="12.69140625" style="9" customWidth="1"/>
+    <col min="10" max="11" width="12.69140625" customWidth="1"/>
+    <col min="12" max="13" width="12.69140625" style="2" customWidth="1"/>
+    <col min="14" max="15" width="12.69140625" customWidth="1"/>
+    <col min="16" max="17" width="12.69140625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="12.69140625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="12.69140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" s="5"/>
+      <c r="O1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="E2" s="1">
+        <v>45586</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="E3" s="1">
+        <v>45586</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45586</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.51527777777777772</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45586</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="E6" s="1">
         <v>45586</v>
       </c>
-      <c r="G2" s="2">
-        <v>0.44861111111111113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="F6" s="11">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1">
         <v>45586</v>
       </c>
-      <c r="G3" s="2">
-        <v>0.44861111111111113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="F7" s="11">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1">
         <v>45586</v>
       </c>
-      <c r="G4" s="2">
-        <v>0.51527777777777772</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F8" s="11">
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
         <v>45586</v>
       </c>
-      <c r="G5" s="2">
-        <v>0.55208333333333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F9" s="11">
+        <v>0.8125</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1">
         <v>45586</v>
       </c>
-      <c r="G6" s="2">
-        <v>0.73263888888888884</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="F10" s="11">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1">
         <v>45586</v>
       </c>
-      <c r="G7" s="2">
-        <v>0.74652777777777779</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1">
-        <v>45586</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.80555555555555558</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="1">
-        <v>45586</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1">
-        <v>45586</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.87708333333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1">
-        <v>45586</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="F11" s="11">
         <v>0.8833333333333333</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A13">
+      <c r="J11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="E12" s="1"/>
+      <c r="J12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -1234,33 +1285,47 @@
       <c r="C13" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="1">
+      <c r="E13" s="1">
         <v>45592</v>
       </c>
-      <c r="G13" s="2">
+      <c r="F13" s="11">
         <v>0.71111111111111114</v>
       </c>
-      <c r="I13" s="3">
+      <c r="G13">
+        <v>29</v>
+      </c>
+      <c r="H13" s="9">
         <v>0.88</v>
       </c>
-      <c r="J13" s="3">
+      <c r="I13" s="9">
         <v>0.7</v>
       </c>
-      <c r="L13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="3">
+      <c r="J13" s="3"/>
+      <c r="K13">
+        <v>39</v>
+      </c>
+      <c r="L13" s="2">
         <v>0.86</v>
       </c>
-      <c r="N13" s="3">
+      <c r="M13" s="2">
         <v>0.66</v>
       </c>
-      <c r="S13" s="4">
+      <c r="N13" s="3"/>
+      <c r="O13">
+        <v>41</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0.91</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="R13" s="11">
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A14">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -1269,15 +1334,47 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="2">
+      <c r="E14" s="1">
+        <v>45592</v>
+      </c>
+      <c r="F14" s="11">
         <v>0.77777777777777779</v>
       </c>
-      <c r="H14">
+      <c r="G14">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A15">
+      <c r="H14" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14">
+        <v>39</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14">
+        <v>41</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="R14" s="11">
+        <v>0.83194444444444449</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1286,12 +1383,47 @@
       <c r="C15" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="2">
+      <c r="E15" s="1">
+        <v>45592</v>
+      </c>
+      <c r="F15" s="11">
         <v>0.8354166666666667</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A16">
+      <c r="G15">
+        <v>39</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.94</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15">
+        <v>41</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15">
+        <v>39</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="R15" s="11">
+        <v>0.89097222222222228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1300,12 +1432,47 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="2">
+      <c r="E16" s="1">
+        <v>45592</v>
+      </c>
+      <c r="F16" s="11">
         <v>0.89166666666666672</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A17">
+      <c r="G16">
+        <v>38</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.91</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16">
+        <v>41</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16">
+        <v>41</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="R16" s="11">
+        <v>0.94513888888888886</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -1314,12 +1481,47 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="2">
+      <c r="E17" s="1">
+        <v>45592</v>
+      </c>
+      <c r="F17" s="11">
         <v>0.94930555555555551</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A18">
+      <c r="G17">
+        <v>38</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17">
+        <v>41</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17">
+        <v>41</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0.83</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>0.53</v>
+      </c>
+      <c r="R17" s="11">
+        <v>3.472222222222222E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A18" s="13">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1328,15 +1530,47 @@
       <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="1">
+      <c r="E18" s="1">
         <v>45593</v>
       </c>
-      <c r="G18" s="2">
+      <c r="F18" s="11">
         <v>6.2500000000000003E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A19">
+      <c r="G18">
+        <v>39</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.81</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18">
+        <v>41</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18">
+        <v>41</v>
+      </c>
+      <c r="P18" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="R18" s="11">
+        <v>5.9027777777777776E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A19" s="13">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1345,12 +1579,47 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="2">
+      <c r="E19" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F19" s="11">
         <v>0.39305555555555555</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A20">
+      <c r="G19">
+        <v>29</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.88</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19">
+        <v>37</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19">
+        <v>39</v>
+      </c>
+      <c r="P19" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R19" s="11">
+        <v>0.44722222222222224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A20" s="13">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1359,15 +1628,47 @@
       <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="2">
+      <c r="E20" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F20" s="11">
         <v>0.57361111111111107</v>
       </c>
-      <c r="S20" s="2">
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20">
+        <v>38</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20">
+        <v>36</v>
+      </c>
+      <c r="P20" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="R20" s="11">
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A21">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A21" s="13">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1376,12 +1677,47 @@
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="2">
+      <c r="E21" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F21" s="11">
         <v>0.64513888888888893</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A22">
+      <c r="G21">
+        <v>33</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21">
+        <v>38</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21">
+        <v>39</v>
+      </c>
+      <c r="P21" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="R21" s="11">
+        <v>0.7006944444444444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A22" s="13">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1390,15 +1726,47 @@
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="2">
+      <c r="E22" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F22" s="11">
         <v>0.70763888888888893</v>
       </c>
-      <c r="S22" s="2">
+      <c r="G22">
+        <v>36</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0.69</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22">
+        <v>38</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22">
+        <v>39</v>
+      </c>
+      <c r="P22" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="R22" s="11">
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A23">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A23" s="13">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1407,15 +1775,47 @@
       <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="2">
+      <c r="E23" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F23" s="11">
         <v>0.76180555555555551</v>
       </c>
-      <c r="S23" s="2">
-        <v>0.31527777777777777</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A24">
+      <c r="G23">
+        <v>38</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23">
+        <v>39</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23">
+        <v>39</v>
+      </c>
+      <c r="P23" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>0.43</v>
+      </c>
+      <c r="R23" s="11">
+        <v>0.81527777777777777</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A24" s="13">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1424,12 +1824,47 @@
       <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="2">
+      <c r="E24" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F24" s="11">
         <v>0.83125000000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A25">
+      <c r="G24">
+        <v>34</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0.67</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0.43</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24">
+        <v>39</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24">
+        <v>39</v>
+      </c>
+      <c r="P24" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0.47</v>
+      </c>
+      <c r="R24" s="11">
+        <v>0.88472222222222219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A25" s="13">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1438,12 +1873,51 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="2">
+      <c r="E25" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F25" s="11">
         <v>0.93055555555555558</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A27">
+      <c r="G25">
+        <v>37</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25">
+        <v>39</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25">
+        <v>40</v>
+      </c>
+      <c r="P25" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="R25" s="11">
+        <v>0.98472222222222228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="J26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A27" s="13">
         <v>24</v>
       </c>
       <c r="B27" t="s">
@@ -1452,15 +1926,47 @@
       <c r="C27" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="1">
+      <c r="E27" s="1">
         <v>45598</v>
       </c>
-      <c r="G27" s="2">
+      <c r="F27" s="11">
         <v>0.50416666666666665</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A28">
+      <c r="G27">
+        <v>27</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27">
+        <v>37</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27">
+        <v>39</v>
+      </c>
+      <c r="P27" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="R27" s="11">
+        <v>0.55902777777777779</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A28" s="13">
         <v>25</v>
       </c>
       <c r="B28" t="s">
@@ -1469,12 +1975,47 @@
       <c r="C28" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="2">
+      <c r="E28" s="1">
+        <v>45598</v>
+      </c>
+      <c r="F28" s="11">
         <v>0.5708333333333333</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A29">
+      <c r="G28">
+        <v>34</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28">
+        <v>39</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28">
+        <v>39</v>
+      </c>
+      <c r="P28" s="7">
+        <v>0.61</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="R28" s="11">
+        <v>0.62430555555555556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A29" s="13">
         <v>26</v>
       </c>
       <c r="B29" t="s">
@@ -1483,12 +2024,47 @@
       <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="2">
+      <c r="E29" s="1">
+        <v>45598</v>
+      </c>
+      <c r="F29" s="11">
         <v>0.63611111111111107</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A30">
+      <c r="G29">
+        <v>35</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29">
+        <v>39</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29">
+        <v>37</v>
+      </c>
+      <c r="P29" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="R29" s="11">
+        <v>0.68888888888888888</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A30" s="13">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -1497,12 +2073,47 @@
       <c r="C30" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="2">
+      <c r="E30" s="1">
+        <v>45598</v>
+      </c>
+      <c r="F30" s="11">
         <v>0.68958333333333333</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A31">
+      <c r="G30">
+        <v>35</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30">
+        <v>37</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30">
+        <v>39</v>
+      </c>
+      <c r="P30" s="7">
+        <v>0.62</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="R30" s="11">
+        <v>0.74652777777777779</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A31" s="13">
         <v>28</v>
       </c>
       <c r="B31" t="s">
@@ -1511,15 +2122,47 @@
       <c r="C31" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="1">
+      <c r="E31" s="1">
         <v>45599</v>
       </c>
-      <c r="G31" s="2">
+      <c r="F31" s="11">
         <v>0.62222222222222223</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A32">
+      <c r="G31">
+        <v>27</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31">
+        <v>37</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31">
+        <v>39</v>
+      </c>
+      <c r="P31" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="R31" s="11">
+        <v>0.67500000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A32" s="13">
         <v>29</v>
       </c>
       <c r="B32" t="s">
@@ -1528,12 +2171,47 @@
       <c r="C32" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="2">
+      <c r="E32" s="1">
+        <v>45599</v>
+      </c>
+      <c r="F32" s="11">
         <v>0.68333333333333335</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33">
+      <c r="G32">
+        <v>35</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0.22</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0.22</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32">
+        <v>39</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32">
+        <v>39</v>
+      </c>
+      <c r="P32" s="7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="R32" s="11">
+        <v>0.73750000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A33" s="13">
         <v>30</v>
       </c>
       <c r="B33" t="s">
@@ -1542,49 +2220,66 @@
       <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="2">
+      <c r="E33" s="1">
+        <v>45599</v>
+      </c>
+      <c r="F33" s="11">
         <v>0.73958333333333337</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I44" s="2"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I46" s="2"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I48" s="2"/>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="I50" s="2"/>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="H52" s="1"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="H54" s="1"/>
-      <c r="I54" s="2"/>
-    </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="H56" s="1"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="H58" s="1"/>
-      <c r="I58" s="2"/>
-    </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="H60" s="1"/>
-      <c r="I60" s="2"/>
-    </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.4">
-      <c r="H62" s="1"/>
-      <c r="I62" s="2"/>
+      <c r="G33">
+        <v>37</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33">
+        <v>40</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33">
+        <v>40</v>
+      </c>
+      <c r="P33" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>0.43</v>
+      </c>
+      <c r="R33" s="11">
+        <v>0.79097222222222219</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G52" s="1"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G62" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
-    <sortCondition ref="F2:F11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+    <sortCondition ref="E2:E11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Tensile Specimen Information
</commit_message>
<xml_diff>
--- a/Randomize-Prints/Tensile-Specimen/Established_Printing_Order.xlsx
+++ b/Randomize-Prints/Tensile-Specimen/Established_Printing_Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berkeley\Documents\GitHub\3D-Filament-Dyes\Randomize-Prints\Tensile-Specimen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C04707-B57A-4174-BD57-AF10E64D251A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1D05BE-EF7B-40C8-965C-ED84E294C45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{26A5D843-55D7-43C2-8BE2-8D2709DF1008}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>green_230</t>
   </si>
@@ -117,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -609,7 +609,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -624,15 +624,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1015,19 +1011,19 @@
   <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="6" max="6" width="12.69140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="12.69140625" style="9" customWidth="1"/>
     <col min="7" max="7" width="12.69140625" customWidth="1"/>
-    <col min="8" max="9" width="12.69140625" style="9" customWidth="1"/>
+    <col min="8" max="9" width="12.69140625" style="7" customWidth="1"/>
     <col min="10" max="11" width="12.69140625" customWidth="1"/>
     <col min="12" max="13" width="12.69140625" style="2" customWidth="1"/>
     <col min="14" max="15" width="12.69140625" customWidth="1"/>
     <col min="16" max="17" width="12.69140625" style="7" customWidth="1"/>
-    <col min="18" max="18" width="12.69140625" style="11" customWidth="1"/>
+    <col min="18" max="18" width="12.69140625" style="9" customWidth="1"/>
     <col min="19" max="19" width="12.69140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1044,26 +1040,26 @@
       <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="N1" s="5"/>
@@ -1076,12 +1072,12 @@
       <c r="Q1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="13">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1093,14 +1089,14 @@
       <c r="E2" s="1">
         <v>45586</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="9">
         <v>0.44861111111111113</v>
       </c>
       <c r="J2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="13">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1112,14 +1108,14 @@
       <c r="E3" s="1">
         <v>45586</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>0.44861111111111113</v>
       </c>
       <c r="J3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1131,14 +1127,14 @@
       <c r="E4" s="1">
         <v>45586</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>0.51527777777777772</v>
       </c>
       <c r="J4" s="3"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="13">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1150,14 +1146,14 @@
       <c r="E5" s="1">
         <v>45586</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>0.55208333333333337</v>
       </c>
       <c r="J5" s="3"/>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1169,14 +1165,14 @@
       <c r="E6" s="1">
         <v>45586</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0.73263888888888884</v>
       </c>
       <c r="J6" s="3"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1188,14 +1184,14 @@
       <c r="E7" s="1">
         <v>45586</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>0.74652777777777779</v>
       </c>
       <c r="J7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1207,14 +1203,14 @@
       <c r="E8" s="1">
         <v>45586</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <v>0.80555555555555558</v>
       </c>
       <c r="J8" s="3"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1226,14 +1222,14 @@
       <c r="E9" s="1">
         <v>45586</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>0.8125</v>
       </c>
       <c r="J9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" s="13">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1245,14 +1241,14 @@
       <c r="E10" s="1">
         <v>45586</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <v>0.87708333333333333</v>
       </c>
       <c r="J10" s="3"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="13">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1264,7 +1260,7 @@
       <c r="E11" s="1">
         <v>45586</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <v>0.8833333333333333</v>
       </c>
       <c r="J11" s="3"/>
@@ -1276,7 +1272,7 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -1288,16 +1284,16 @@
       <c r="E13" s="1">
         <v>45592</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <v>0.71111111111111114</v>
       </c>
       <c r="G13">
         <v>29</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>0.88</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="7">
         <v>0.7</v>
       </c>
       <c r="J13" s="3"/>
@@ -1320,12 +1316,12 @@
       <c r="Q13" s="7">
         <v>0.7</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="9">
         <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -1337,16 +1333,16 @@
       <c r="E14" s="1">
         <v>45592</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>0.77777777777777779</v>
       </c>
       <c r="G14">
         <v>37</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <v>0.9</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <v>0.68</v>
       </c>
       <c r="J14" s="3"/>
@@ -1369,12 +1365,12 @@
       <c r="Q14" s="7">
         <v>0.65</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="9">
         <v>0.83194444444444449</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1386,16 +1382,16 @@
       <c r="E15" s="1">
         <v>45592</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <v>0.8354166666666667</v>
       </c>
       <c r="G15">
         <v>39</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <v>0.94</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>0.68</v>
       </c>
       <c r="J15" s="3"/>
@@ -1418,12 +1414,12 @@
       <c r="Q15" s="7">
         <v>0.68</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="9">
         <v>0.89097222222222228</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="13">
+      <c r="A16" s="11">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1435,16 +1431,16 @@
       <c r="E16" s="1">
         <v>45592</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <v>0.89166666666666672</v>
       </c>
       <c r="G16">
         <v>38</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="7">
         <v>0.91</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="7">
         <v>0.63</v>
       </c>
       <c r="J16" s="3"/>
@@ -1467,12 +1463,12 @@
       <c r="Q16" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="9">
         <v>0.94513888888888886</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" s="13">
+      <c r="A17" s="11">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -1484,16 +1480,16 @@
       <c r="E17" s="1">
         <v>45592</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>0.94930555555555551</v>
       </c>
       <c r="G17">
         <v>38</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="7">
         <v>0.74</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <v>0.49</v>
       </c>
       <c r="J17" s="3"/>
@@ -1516,12 +1512,12 @@
       <c r="Q17" s="7">
         <v>0.53</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="9">
         <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1533,16 +1529,16 @@
       <c r="E18" s="1">
         <v>45593</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="G18">
         <v>39</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>0.81</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="7">
         <v>0.51</v>
       </c>
       <c r="J18" s="3"/>
@@ -1565,12 +1561,12 @@
       <c r="Q18" s="7">
         <v>0.48</v>
       </c>
-      <c r="R18" s="11">
+      <c r="R18" s="9">
         <v>5.9027777777777776E-2</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A19" s="13">
+      <c r="A19" s="11">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1582,16 +1578,16 @@
       <c r="E19" s="1">
         <v>45593</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="9">
         <v>0.39305555555555555</v>
       </c>
       <c r="G19">
         <v>29</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="7">
         <v>0.88</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="7">
         <v>0.56999999999999995</v>
       </c>
       <c r="J19" s="3"/>
@@ -1614,12 +1610,12 @@
       <c r="Q19" s="7">
         <v>0.56000000000000005</v>
       </c>
-      <c r="R19" s="11">
+      <c r="R19" s="9">
         <v>0.44722222222222224</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A20" s="13">
+      <c r="A20" s="11">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1631,16 +1627,16 @@
       <c r="E20" s="1">
         <v>45593</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="9">
         <v>0.57361111111111107</v>
       </c>
       <c r="G20">
         <v>30</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="7">
         <v>0.75</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="7">
         <v>0.62</v>
       </c>
       <c r="J20" s="3"/>
@@ -1663,12 +1659,12 @@
       <c r="Q20" s="7">
         <v>0.56999999999999995</v>
       </c>
-      <c r="R20" s="11">
+      <c r="R20" s="9">
         <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A21" s="13">
+      <c r="A21" s="11">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1680,16 +1676,16 @@
       <c r="E21" s="1">
         <v>45593</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="9">
         <v>0.64513888888888893</v>
       </c>
       <c r="G21">
         <v>33</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="7">
         <v>0.75</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="7">
         <v>0.6</v>
       </c>
       <c r="J21" s="3"/>
@@ -1712,12 +1708,12 @@
       <c r="Q21" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="R21" s="11">
+      <c r="R21" s="9">
         <v>0.7006944444444444</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A22" s="13">
+      <c r="A22" s="11">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1729,16 +1725,16 @@
       <c r="E22" s="1">
         <v>45593</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="9">
         <v>0.70763888888888893</v>
       </c>
       <c r="G22">
         <v>36</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="7">
         <v>0.69</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="7">
         <v>0.55000000000000004</v>
       </c>
       <c r="J22" s="3"/>
@@ -1761,12 +1757,12 @@
       <c r="Q22" s="7">
         <v>0.54</v>
       </c>
-      <c r="R22" s="11">
+      <c r="R22" s="9">
         <v>0.26041666666666669</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1778,16 +1774,16 @@
       <c r="E23" s="1">
         <v>45593</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="9">
         <v>0.76180555555555551</v>
       </c>
       <c r="G23">
         <v>38</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="7">
         <v>0.66</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="7">
         <v>0.48</v>
       </c>
       <c r="J23" s="3"/>
@@ -1810,12 +1806,12 @@
       <c r="Q23" s="7">
         <v>0.43</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="9">
         <v>0.81527777777777777</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A24" s="13">
+      <c r="A24" s="11">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1827,16 +1823,16 @@
       <c r="E24" s="1">
         <v>45593</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="9">
         <v>0.83125000000000004</v>
       </c>
       <c r="G24">
         <v>34</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="7">
         <v>0.67</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="7">
         <v>0.43</v>
       </c>
       <c r="J24" s="3"/>
@@ -1859,12 +1855,12 @@
       <c r="Q24" s="7">
         <v>0.47</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="9">
         <v>0.88472222222222219</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="A25" s="11">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1876,16 +1872,16 @@
       <c r="E25" s="1">
         <v>45593</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="9">
         <v>0.93055555555555558</v>
       </c>
       <c r="G25">
         <v>37</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="7">
         <v>0.74</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="7">
         <v>0.44</v>
       </c>
       <c r="J25" s="3"/>
@@ -1908,7 +1904,7 @@
       <c r="Q25" s="7">
         <v>0.45</v>
       </c>
-      <c r="R25" s="11">
+      <c r="R25" s="9">
         <v>0.98472222222222228</v>
       </c>
     </row>
@@ -1917,7 +1913,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A27" s="13">
+      <c r="A27" s="11">
         <v>24</v>
       </c>
       <c r="B27" t="s">
@@ -1929,16 +1925,16 @@
       <c r="E27" s="1">
         <v>45598</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="9">
         <v>0.50416666666666665</v>
       </c>
       <c r="G27">
         <v>27</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="7">
         <v>0.59</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="7">
         <v>0.45</v>
       </c>
       <c r="J27" s="3"/>
@@ -1961,12 +1957,12 @@
       <c r="Q27" s="7">
         <v>0.45</v>
       </c>
-      <c r="R27" s="11">
+      <c r="R27" s="9">
         <v>0.55902777777777779</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A28" s="13">
+      <c r="A28" s="11">
         <v>25</v>
       </c>
       <c r="B28" t="s">
@@ -1978,16 +1974,16 @@
       <c r="E28" s="1">
         <v>45598</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="9">
         <v>0.5708333333333333</v>
       </c>
       <c r="G28">
         <v>34</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="7">
         <v>0.64</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="7">
         <v>0.5</v>
       </c>
       <c r="J28" s="3"/>
@@ -2010,12 +2006,12 @@
       <c r="Q28" s="7">
         <v>0.49</v>
       </c>
-      <c r="R28" s="11">
+      <c r="R28" s="9">
         <v>0.62430555555555556</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A29" s="13">
+      <c r="A29" s="11">
         <v>26</v>
       </c>
       <c r="B29" t="s">
@@ -2027,16 +2023,16 @@
       <c r="E29" s="1">
         <v>45598</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="9">
         <v>0.63611111111111107</v>
       </c>
       <c r="G29">
         <v>35</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="7">
         <v>0.48</v>
       </c>
       <c r="J29" s="3"/>
@@ -2059,12 +2055,12 @@
       <c r="Q29" s="7">
         <v>0.49</v>
       </c>
-      <c r="R29" s="11">
+      <c r="R29" s="9">
         <v>0.68888888888888888</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A30" s="13">
+      <c r="A30" s="11">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -2076,16 +2072,16 @@
       <c r="E30" s="1">
         <v>45598</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="9">
         <v>0.68958333333333333</v>
       </c>
       <c r="G30">
         <v>35</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="7">
         <v>0.6</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="7">
         <v>0.49</v>
       </c>
       <c r="J30" s="3"/>
@@ -2108,12 +2104,12 @@
       <c r="Q30" s="7">
         <v>0.46</v>
       </c>
-      <c r="R30" s="11">
+      <c r="R30" s="9">
         <v>0.74652777777777779</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A31" s="13">
+      <c r="A31" s="11">
         <v>28</v>
       </c>
       <c r="B31" t="s">
@@ -2125,16 +2121,16 @@
       <c r="E31" s="1">
         <v>45599</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="9">
         <v>0.62222222222222223</v>
       </c>
       <c r="G31">
         <v>27</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="7">
         <v>0.26</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="7">
         <v>0.26</v>
       </c>
       <c r="J31" s="3"/>
@@ -2157,12 +2153,12 @@
       <c r="Q31" s="7">
         <v>0.2</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="9">
         <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A32" s="13">
+      <c r="A32" s="11">
         <v>29</v>
       </c>
       <c r="B32" t="s">
@@ -2174,16 +2170,16 @@
       <c r="E32" s="1">
         <v>45599</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="9">
         <v>0.68333333333333335</v>
       </c>
       <c r="G32">
         <v>35</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="7">
         <v>0.22</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="7">
         <v>0.22</v>
       </c>
       <c r="J32" s="3"/>
@@ -2206,12 +2202,12 @@
       <c r="Q32" s="7">
         <v>0.41</v>
       </c>
-      <c r="R32" s="11">
+      <c r="R32" s="9">
         <v>0.73750000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A33" s="13">
+      <c r="A33" s="11">
         <v>30</v>
       </c>
       <c r="B33" t="s">
@@ -2223,16 +2219,16 @@
       <c r="E33" s="1">
         <v>45599</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="9">
         <v>0.73958333333333337</v>
       </c>
       <c r="G33">
         <v>37</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I33" s="7">
         <v>0.4</v>
       </c>
       <c r="J33" s="3"/>
@@ -2255,7 +2251,7 @@
       <c r="Q33" s="7">
         <v>0.43</v>
       </c>
-      <c r="R33" s="11">
+      <c r="R33" s="9">
         <v>0.79097222222222219</v>
       </c>
     </row>

</xml_diff>